<commit_message>
Did some more work
</commit_message>
<xml_diff>
--- a/Experimente.xlsx
+++ b/Experimente.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyrill Marti\Desktop\PhysikLaborMotoren\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyrill.Marti\Desktop\PhysikLaborMotoren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0A1082-D1BA-47E0-A82E-680C6E0950E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BE1658-E02A-408C-AD42-CB50D96FBC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Exp. 1</t>
   </si>
@@ -103,6 +103,18 @@
   <si>
     <t>deltas (rad)</t>
   </si>
+  <si>
+    <t>omega (rad/frame)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Exp. 4</t>
+  </si>
+  <si>
+    <t>Drehmoment</t>
+  </si>
 </sst>
 </file>
 
@@ -162,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -180,7 +192,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -247,7 +259,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -422,7 +434,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -460,7 +472,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1179304975"/>
@@ -545,7 +557,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -583,7 +595,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="991709903"/>
@@ -631,7 +643,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -645,7 +657,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -714,7 +726,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -923,7 +935,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -961,7 +973,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="316344400"/>
@@ -1040,7 +1052,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1078,7 +1090,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="314284672"/>
@@ -1126,7 +1138,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1140,7 +1152,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1207,7 +1219,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1220,8 +1232,49 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$40:$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1286,7 +1339,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$F$40:$F$50</c:f>
+              <c:f>Tabelle1!$G$40:$G$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1294,34 +1347,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1693705988362009E-2</c:v>
+                  <c:v>2.338741197672402E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27052603405912112</c:v>
+                  <c:v>5.4105206811824222E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1313224211427244</c:v>
+                  <c:v>0.22626448422854489</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.91018920491504263</c:v>
+                  <c:v>0.18203784098300851</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0595893888857577</c:v>
+                  <c:v>0.21191787777715154</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4603169851436553</c:v>
+                  <c:v>0.29206339702873108</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4460052852773027</c:v>
+                  <c:v>0.28920105705546051</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6210618092523328</c:v>
+                  <c:v>0.32421236185046653</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3941690064930699</c:v>
+                  <c:v>0.27883380129861396</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6427038919770638</c:v>
+                  <c:v>0.32854077839541274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1329,7 +1382,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B325-4F42-AF38-172378A576FF}"/>
+              <c16:uniqueId val="{00000000-42CA-4B98-832C-84DE39CF5554}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1416,7 +1469,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1454,7 +1507,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="316342912"/>
@@ -1533,7 +1586,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1571,7 +1624,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2064657072"/>
@@ -1619,7 +1672,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3551,13 +3604,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>34050</xdr:colOff>
+      <xdr:colOff>596025</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>15343</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>370225</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>322600</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>91543</xdr:rowOff>
     </xdr:to>
@@ -3586,14 +3639,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>410307</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>362682</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>20516</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>117230</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>69605</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>96716</xdr:rowOff>
     </xdr:to>
@@ -3886,13 +3939,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V50"/>
+  <dimension ref="A1:V129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V35" sqref="V35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4073,17 +4126,17 @@
         <v>98.274445357436321</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>24</v>
       </c>
@@ -4099,8 +4152,11 @@
       <c r="F39" t="s">
         <v>21</v>
       </c>
+      <c r="G39" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>0</v>
       </c>
@@ -4115,8 +4171,12 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="G40">
+        <f>F40/5</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>5</v>
       </c>
@@ -4125,15 +4185,19 @@
         <v>0.67</v>
       </c>
       <c r="E41">
-        <f t="shared" ref="E41:E50" si="1">D41*(PI()/180)</f>
+        <f t="shared" ref="E41:E49" si="1">D41*(PI()/180)</f>
         <v>1.1693705988362009E-2</v>
       </c>
       <c r="F41">
         <f>E41-E40</f>
         <v>1.1693705988362009E-2</v>
       </c>
+      <c r="G41">
+        <f t="shared" ref="G41:G50" si="2">F41/5</f>
+        <v>2.338741197672402E-3</v>
+      </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>10</v>
       </c>
@@ -4146,11 +4210,15 @@
         <v>0.28221974004748313</v>
       </c>
       <c r="F42">
-        <f t="shared" ref="F42:F50" si="2">E42-E41</f>
+        <f t="shared" ref="F42:F50" si="3">E42-E41</f>
         <v>0.27052603405912112</v>
       </c>
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>5.4105206811824222E-2</v>
+      </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>15</v>
       </c>
@@ -4163,11 +4231,15 @@
         <v>1.4135421611902075</v>
       </c>
       <c r="F43">
+        <f t="shared" si="3"/>
+        <v>1.1313224211427244</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="2"/>
-        <v>1.1313224211427244</v>
+        <v>0.22626448422854489</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>20</v>
       </c>
@@ -4180,11 +4252,15 @@
         <v>2.3237313661052501</v>
       </c>
       <c r="F44">
+        <f t="shared" si="3"/>
+        <v>0.91018920491504263</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="2"/>
-        <v>0.91018920491504263</v>
+        <v>0.18203784098300851</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>25</v>
       </c>
@@ -4197,11 +4273,15 @@
         <v>3.3833207549910078</v>
       </c>
       <c r="F45">
+        <f t="shared" si="3"/>
+        <v>1.0595893888857577</v>
+      </c>
+      <c r="G45">
         <f t="shared" si="2"/>
-        <v>1.0595893888857577</v>
+        <v>0.21191787777715154</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>30</v>
       </c>
@@ -4214,11 +4294,15 @@
         <v>4.8436377401346631</v>
       </c>
       <c r="F46">
+        <f t="shared" si="3"/>
+        <v>1.4603169851436553</v>
+      </c>
+      <c r="G46">
         <f t="shared" si="2"/>
-        <v>1.4603169851436553</v>
+        <v>0.29206339702873108</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>35</v>
       </c>
@@ -4231,11 +4315,15 @@
         <v>6.2896430254119657</v>
       </c>
       <c r="F47">
+        <f t="shared" si="3"/>
+        <v>1.4460052852773027</v>
+      </c>
+      <c r="G47">
         <f t="shared" si="2"/>
-        <v>1.4460052852773027</v>
+        <v>0.28920105705546051</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>40</v>
       </c>
@@ -4248,11 +4336,15 @@
         <v>7.9107048346642985</v>
       </c>
       <c r="F48">
+        <f t="shared" si="3"/>
+        <v>1.6210618092523328</v>
+      </c>
+      <c r="G48">
         <f t="shared" si="2"/>
-        <v>1.6210618092523328</v>
+        <v>0.32421236185046653</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>45</v>
       </c>
@@ -4265,11 +4357,15 @@
         <v>9.3048738411573684</v>
       </c>
       <c r="F49">
+        <f t="shared" si="3"/>
+        <v>1.3941690064930699</v>
+      </c>
+      <c r="G49">
         <f t="shared" si="2"/>
-        <v>1.3941690064930699</v>
+        <v>0.27883380129861396</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>50</v>
       </c>
@@ -4282,8 +4378,50 @@
         <v>10.947577733134432</v>
       </c>
       <c r="F50">
+        <f t="shared" si="3"/>
+        <v>1.6427038919770638</v>
+      </c>
+      <c r="G50">
         <f t="shared" si="2"/>
-        <v>1.6427038919770638</v>
+        <v>0.32854077839541274</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>